<commit_message>
big update, app is now being developed on mobile device -mobile controls implemented -database loading on mobile device has been fixed
</commit_message>
<xml_diff>
--- a/block-diagrams/RequestedArtAssets.xlsx
+++ b/block-diagrams/RequestedArtAssets.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sasha\Desktop\space game\space-game\block-diagrams\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\damie\OneDrive\Documents\Hobby Stuff\UnityProjects\space-game\block-diagrams\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A10238B3-9F80-4B01-9297-8B4177B75602}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8A1C1F0-FE9B-40E2-BBA9-148CF2918C64}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="33">
   <si>
     <t xml:space="preserve">Sprite </t>
   </si>
@@ -109,6 +109,21 @@
   </si>
   <si>
     <t>Sasha</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>Security Table</t>
+  </si>
+  <si>
+    <t xml:space="preserve">a table with monitors, for viewing security camera footage </t>
+  </si>
+  <si>
+    <t>Chair</t>
+  </si>
+  <si>
+    <t xml:space="preserve">a chair for tables </t>
   </si>
 </sst>
 </file>
@@ -435,10 +450,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D20"/>
+  <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -486,6 +501,9 @@
       <c r="C7" t="s">
         <v>27</v>
       </c>
+      <c r="D7" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -494,6 +512,12 @@
       <c r="B8" t="s">
         <v>7</v>
       </c>
+      <c r="C8" t="s">
+        <v>27</v>
+      </c>
+      <c r="D8" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
@@ -505,30 +529,36 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>26</v>
+        <v>29</v>
+      </c>
+      <c r="B10" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>19</v>
+      <c r="A11" t="s">
+        <v>31</v>
+      </c>
+      <c r="B11" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>9</v>
-      </c>
-      <c r="B12" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>11</v>
+      <c r="A13" s="1" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>10</v>
+        <v>9</v>
+      </c>
+      <c r="B14" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -538,35 +568,45 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
-        <v>18</v>
+      <c r="A17" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>4</v>
-      </c>
-      <c r="B18" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>13</v>
-      </c>
-      <c r="B19" t="s">
-        <v>14</v>
+      <c r="A19" s="1" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
+        <v>4</v>
+      </c>
+      <c r="B20" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>13</v>
+      </c>
+      <c r="B21" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>16</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B22" t="s">
         <v>17</v>
       </c>
     </row>

</xml_diff>